<commit_message>
Tap mit Bug-Liste hinzugefügt
</commit_message>
<xml_diff>
--- a/Projekt Dokumente/Projektsteuerung.xlsx
+++ b/Projekt Dokumente/Projektsteuerung.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SD_Card/HSR/D2D/Projekt Dokumente/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14160" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitefassung" sheetId="1" r:id="rId1"/>
@@ -17,24 +12,22 @@
     <sheet name="Todos" sheetId="3" r:id="rId3"/>
     <sheet name="Use Cases" sheetId="5" r:id="rId4"/>
     <sheet name="Anforderungen" sheetId="4" r:id="rId5"/>
+    <sheet name="Bugs" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="100">
   <si>
     <t>Wer</t>
   </si>
@@ -310,6 +303,30 @@
   </si>
   <si>
     <t>File.IO Service</t>
+  </si>
+  <si>
+    <t>Android Receive Shared File</t>
+  </si>
+  <si>
+    <t>Dokumentation</t>
+  </si>
+  <si>
+    <t>Der Benutzer überträgt eine Datei in die Cloud und kann den Link per  angezeigtem QR-Code einer weitern Person zur verfügung stellen</t>
+  </si>
+  <si>
+    <t>Der Benutzer kann den QR-Code einer anderen Person scannen und die Verknüpfte Datei aus der Cloud herunter landen und sie danach mit anderen Apps teilen.</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>Finder</t>
+  </si>
+  <si>
+    <t>App stürzt ab wenn versucht wird zu scannen und keine Kamera vorhanden ist.</t>
   </si>
 </sst>
 </file>
@@ -393,7 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -431,68 +448,101 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="31">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="d/mm/yy;@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -524,52 +574,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A2:E57" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A2:E57" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A2:E57"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Wer" dataDxfId="21"/>
-    <tableColumn id="2" name="Was" dataDxfId="20"/>
-    <tableColumn id="6" name="Typ" dataDxfId="19"/>
-    <tableColumn id="3" name="Wann" dataDxfId="0"/>
-    <tableColumn id="4" name="Dauer [h]" dataDxfId="18"/>
+    <tableColumn id="1" name="Wer" dataDxfId="28"/>
+    <tableColumn id="2" name="Was" dataDxfId="27"/>
+    <tableColumn id="6" name="Typ" dataDxfId="26"/>
+    <tableColumn id="3" name="Wann" dataDxfId="25"/>
+    <tableColumn id="4" name="Dauer [h]" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A2:D25" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A2:D25" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A2:D25"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Was" dataDxfId="15"/>
-    <tableColumn id="3" name="Typ" dataDxfId="14"/>
-    <tableColumn id="5" name="Status" dataDxfId="13"/>
-    <tableColumn id="4" name="Wer" dataDxfId="12"/>
+    <tableColumn id="1" name="Was" dataDxfId="21"/>
+    <tableColumn id="3" name="Typ" dataDxfId="20"/>
+    <tableColumn id="5" name="Status" dataDxfId="19"/>
+    <tableColumn id="4" name="Wer" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A2:B24" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A2:B24" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A2:B24"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Name" dataDxfId="9"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="8"/>
+    <tableColumn id="1" name="Name" dataDxfId="15"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:E24" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:E24" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A2:E24"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="5"/>
-    <tableColumn id="2" name="Muss/Soll/Kann" dataDxfId="4"/>
-    <tableColumn id="3" name="Beschreibung" dataDxfId="3"/>
-    <tableColumn id="4" name="Status" dataDxfId="2"/>
-    <tableColumn id="5" name="Bemerkungen" dataDxfId="1"/>
+    <tableColumn id="1" name="#" dataDxfId="11"/>
+    <tableColumn id="2" name="Muss/Soll/Kann" dataDxfId="10"/>
+    <tableColumn id="3" name="Beschreibung" dataDxfId="9"/>
+    <tableColumn id="4" name="Status" dataDxfId="8"/>
+    <tableColumn id="5" name="Bemerkungen" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle6" displayName="Tabelle6" ref="A2:E33" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A2:E33"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="#1" dataDxfId="6"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="5"/>
+    <tableColumn id="3" name="Finder" dataDxfId="4"/>
+    <tableColumn id="4" name="Status" dataDxfId="3"/>
+    <tableColumn id="5" name="Bemerkungen" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -874,21 +938,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="14" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="3"/>
+    <col min="4" max="4" width="9.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>26</v>
       </c>
@@ -897,7 +961,7 @@
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -914,13 +978,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -937,7 +1001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -954,7 +1018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -971,7 +1035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -983,7 +1047,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1000,7 +1064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1017,7 +1081,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1034,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1051,7 +1115,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1068,7 +1132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>5</v>
       </c>
@@ -1085,7 +1149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>5</v>
       </c>
@@ -1102,7 +1166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -1119,130 +1183,158 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="7">
+        <v>43071</v>
+      </c>
+      <c r="E16" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="7">
+        <v>43072</v>
+      </c>
+      <c r="E17" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="7"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="7"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="7"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="7"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="7"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="7"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="7"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="7"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="7"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="7"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="7"/>
     </row>
   </sheetData>
@@ -1266,86 +1358,86 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="10.85546875" style="3"/>
+    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
     </row>
-    <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>0.5</v>
       </c>
@@ -1353,7 +1445,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>24</v>
       </c>
@@ -1370,19 +1462,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" style="3" customWidth="1"/>
-    <col min="2" max="3" width="25.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="25.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="21" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="3"/>
+    <col min="5" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>27</v>
       </c>
@@ -1390,7 +1482,7 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1404,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1418,7 +1510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -1432,7 +1524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
@@ -1446,7 +1538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
@@ -1457,7 +1549,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -1465,7 +1557,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>47</v>
       </c>
@@ -1473,7 +1565,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
@@ -1481,7 +1573,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
@@ -1489,12 +1581,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1505,7 +1597,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
@@ -1513,7 +1605,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1524,7 +1616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
@@ -1535,7 +1627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -1546,7 +1638,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -1554,7 +1646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>83</v>
       </c>
@@ -1568,7 +1660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>84</v>
       </c>
@@ -1582,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>85</v>
       </c>
@@ -1613,23 +1705,23 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="77" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="3"/>
+    <col min="3" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
@@ -1637,14 +1729,20 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>81</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1660,26 +1758,26 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="60.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="3"/>
-    <col min="5" max="5" width="22.83203125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="4.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="3"/>
+    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>48</v>
       </c>
@@ -1696,7 +1794,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1707,7 +1805,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1718,7 +1816,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1729,7 +1827,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1740,7 +1838,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1751,7 +1849,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1759,7 +1857,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1770,7 +1868,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1781,7 +1879,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1792,7 +1890,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1803,7 +1901,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1814,7 +1912,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1825,7 +1923,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1836,7 +1934,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1847,7 +1945,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1858,7 +1956,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1869,32 +1967,32 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -1905,4 +2003,62 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="14" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="13"/>
+    <col min="5" max="5" width="15.5703125" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Projektsteuerung. Learnings, Task, Status
</commit_message>
<xml_diff>
--- a/Projekt Dokumente/Projektsteuerung.xlsx
+++ b/Projekt Dokumente/Projektsteuerung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="14160" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="14160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitefassung" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Use Cases" sheetId="5" r:id="rId4"/>
     <sheet name="Anforderungen" sheetId="4" r:id="rId5"/>
     <sheet name="Bugs" sheetId="6" r:id="rId6"/>
+    <sheet name="Erekenntnisse" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="124">
   <si>
     <t>Wer</t>
   </si>
@@ -345,6 +346,63 @@
   </si>
   <si>
     <t>Reto Scherrer</t>
+  </si>
+  <si>
+    <t>Erkenntnisse/LearningsProbleme</t>
+  </si>
+  <si>
+    <t>Testing vernachlässigt, da der zeitliche Aufwand für das erstellen von Mocks als zu gross erachtet wurde im Verhältnis zur zu verfügung stehenden Zeit.</t>
+  </si>
+  <si>
+    <t>Für alle überraschent ist die Tatsache, dass sehr vieles was wir als Grundlegende anforderung an eine App nicht durch Xamarin bereits Platformunabhängig zur Verfügung steht. Zwar ist vieles über Nuget/Githup nachrüstbar. Aber diese Abhängigkeiten führten zu anderen Problemen.</t>
+  </si>
+  <si>
+    <t>Oft funktionierte etwas an der Entwicklungs-Umgebung nicht mehr. Entweder nach einem Update von Visualstudio selber oder eines der Nuget-Packete. Oder aus sonst unerfindlichen Gründen. Preview, Simulator-Start/Debugging. Auf Mac unterschiedlich als zu Windows-PC</t>
+  </si>
+  <si>
+    <t>Ständige Updates von Nuget Packete nötig, verfügbar, inkompatibel. Consolidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertiefung MVVM-Architektur und XAML-Design </t>
+  </si>
+  <si>
+    <t>IDE Updates</t>
+  </si>
+  <si>
+    <t>Update von Xcode auf Version 11.2, Update von Visual Studio, weil ich am Samstag mein iPhone SE auf die neuste aktualisiert habe</t>
+  </si>
+  <si>
+    <t>Erstellung und Verfeinerung des App Icons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umsetzung UI Design </t>
+  </si>
+  <si>
+    <t>Optimierung UI Design</t>
+  </si>
+  <si>
+    <t>Visual Studio Update rückgängig machen, neu Installieren. Simulator nicht mehr verwendbar</t>
+  </si>
+  <si>
+    <t>Statusupdate, Tasks/Probleme besprechen</t>
+  </si>
+  <si>
+    <t>Alle</t>
+  </si>
+  <si>
+    <t>Konzeption</t>
+  </si>
+  <si>
+    <t>User Settings</t>
+  </si>
+  <si>
+    <t>Stauts-Meeting</t>
+  </si>
+  <si>
+    <t>Bestehende Probleme lösen</t>
+  </si>
+  <si>
+    <t>Primärer Use-Case f. Android im UI realisieren</t>
   </si>
 </sst>
 </file>
@@ -428,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -472,11 +530,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -485,6 +552,9 @@
   </cellStyles>
   <dxfs count="31">
     <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -561,9 +631,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="d/mm/yy;@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -592,66 +659,69 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A2:E57" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="A2:E57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A2:E56" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="A2:E56"/>
+  <sortState ref="A3:E56">
+    <sortCondition ref="D2:D56"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" name="Wer" dataDxfId="28"/>
-    <tableColumn id="2" name="Was" dataDxfId="27"/>
-    <tableColumn id="6" name="Typ" dataDxfId="26"/>
-    <tableColumn id="3" name="Wann" dataDxfId="25"/>
-    <tableColumn id="4" name="Dauer [h]" dataDxfId="24"/>
+    <tableColumn id="2" name="Was" dataDxfId="0"/>
+    <tableColumn id="6" name="Typ" dataDxfId="27"/>
+    <tableColumn id="3" name="Wann" dataDxfId="26"/>
+    <tableColumn id="4" name="Dauer [h]" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A2:D25" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A2:D25" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A2:D25"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Was" dataDxfId="21"/>
-    <tableColumn id="3" name="Typ" dataDxfId="20"/>
-    <tableColumn id="5" name="Status" dataDxfId="19"/>
-    <tableColumn id="4" name="Wer" dataDxfId="18"/>
+    <tableColumn id="1" name="Was" dataDxfId="22"/>
+    <tableColumn id="3" name="Typ" dataDxfId="21"/>
+    <tableColumn id="5" name="Status" dataDxfId="20"/>
+    <tableColumn id="4" name="Wer" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A2:B24" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A2:B24" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A2:B24"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Name" dataDxfId="15"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="14"/>
+    <tableColumn id="1" name="Name" dataDxfId="16"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:E24" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:E24" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A2:E24"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="11"/>
-    <tableColumn id="2" name="Muss/Soll/Kann" dataDxfId="10"/>
-    <tableColumn id="3" name="Beschreibung" dataDxfId="9"/>
-    <tableColumn id="4" name="Status" dataDxfId="8"/>
-    <tableColumn id="5" name="Bemerkungen" dataDxfId="7"/>
+    <tableColumn id="1" name="#" dataDxfId="12"/>
+    <tableColumn id="2" name="Muss/Soll/Kann" dataDxfId="11"/>
+    <tableColumn id="3" name="Beschreibung" dataDxfId="10"/>
+    <tableColumn id="4" name="Status" dataDxfId="9"/>
+    <tableColumn id="5" name="Bemerkungen" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle6" displayName="Tabelle6" ref="A2:E33" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle6" displayName="Tabelle6" ref="A2:E33" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A2:E33"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#1" dataDxfId="4"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="3"/>
-    <tableColumn id="3" name="Finder" dataDxfId="2"/>
-    <tableColumn id="4" name="Status" dataDxfId="1"/>
-    <tableColumn id="5" name="Bemerkungen" dataDxfId="0"/>
+    <tableColumn id="1" name="#1" dataDxfId="5"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="4"/>
+    <tableColumn id="3" name="Finder" dataDxfId="3"/>
+    <tableColumn id="4" name="Status" dataDxfId="2"/>
+    <tableColumn id="5" name="Bemerkungen" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -954,17 +1024,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47.3125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16" style="15" customWidth="1"/>
+    <col min="2" max="2" width="47.3125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14" style="15" customWidth="1"/>
     <col min="4" max="4" width="9.68359375" style="3" customWidth="1"/>
     <col min="5" max="5" width="9.83984375" style="3" customWidth="1"/>
     <col min="6" max="16384" width="8.83984375" style="3"/>
@@ -974,19 +1044,19 @@
       <c r="A1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="4"/>
       <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -997,99 +1067,115 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3" t="s">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C3" s="15" t="s">
         <v>56</v>
       </c>
+      <c r="D3" s="7">
+        <v>43052</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>56</v>
+      </c>
       <c r="D4" s="7">
-        <v>43052</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2</v>
+        <v>43053</v>
+      </c>
+      <c r="E4" s="9">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7">
+        <v>43054</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="7">
-        <v>43053</v>
-      </c>
-      <c r="E5" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="15" t="s">
         <v>56</v>
       </c>
       <c r="D6" s="7">
         <v>43059</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="A7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7">
+        <v>43064</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>10</v>
-      </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="D8" s="7">
         <v>43064</v>
       </c>
       <c r="E8" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="A9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="7">
@@ -1100,13 +1186,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="A10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="7">
@@ -1117,98 +1203,98 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="A11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="7">
+        <v>43065</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7">
-        <v>43064</v>
-      </c>
-      <c r="E11" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="3" t="s">
+      <c r="D12" s="7">
+        <v>43069</v>
+      </c>
+      <c r="E12" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D13" s="7">
         <v>43070</v>
-      </c>
-      <c r="E12" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="7">
-        <v>43065</v>
       </c>
       <c r="E13" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>10</v>
+      <c r="B14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="D14" s="7">
-        <v>43069</v>
-      </c>
-      <c r="E14" s="9">
-        <v>3</v>
+        <v>43070</v>
+      </c>
+      <c r="E14" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="A15" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>56</v>
       </c>
       <c r="D15" s="7">
         <v>43070</v>
       </c>
       <c r="E15" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="15" t="s">
         <v>56</v>
       </c>
       <c r="D16" s="7">
@@ -1219,13 +1305,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="15" t="s">
         <v>93</v>
       </c>
       <c r="D17" s="7">
@@ -1235,65 +1321,65 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="7">
+        <v>43072</v>
+      </c>
+      <c r="E18" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="7">
+        <v>43072</v>
+      </c>
+      <c r="E19" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C20" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D20" s="7">
         <v>43073</v>
-      </c>
-      <c r="E18" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="7">
-        <v>43074</v>
-      </c>
-      <c r="E19" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="7">
-        <v>43075</v>
       </c>
       <c r="E20" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="15" t="s">
         <v>56</v>
       </c>
       <c r="D21" s="7">
@@ -1304,45 +1390,157 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="7">
+        <v>43073</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="7">
+        <v>43074</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="7">
+        <v>43074</v>
+      </c>
+      <c r="E24" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="7">
+        <v>43075</v>
+      </c>
+      <c r="E25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="7">
+        <v>43075</v>
+      </c>
+      <c r="E26" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C27" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="7">
-        <v>43046</v>
-      </c>
-      <c r="E22" s="3">
+      <c r="D27" s="7">
+        <v>43076</v>
+      </c>
+      <c r="E27" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D27" s="7"/>
-    </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D28" s="7"/>
+      <c r="A28" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="7">
+        <v>43076</v>
+      </c>
+      <c r="E28" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D29" s="7"/>
+      <c r="A29" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="7">
+        <v>43076</v>
+      </c>
+      <c r="E29" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D30" s="7"/>
+      <c r="A30" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="7">
+        <v>43077</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D31" s="7"/>
@@ -1422,12 +1620,8 @@
     <row r="56" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="D57" s="7"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
+  <mergeCells count="1">
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1442,28 +1636,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="10.83984375" style="3"/>
-    <col min="2" max="2" width="19.68359375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="39.20703125" style="3" customWidth="1"/>
     <col min="3" max="16384" width="10.83984375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
@@ -1505,9 +1699,29 @@
         <v>18</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="13" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1548,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1563,12 +1777,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
@@ -1641,30 +1855,51 @@
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C7" s="8" t="s">
         <v>41</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="B8" s="15" t="s">
+        <v>119</v>
+      </c>
       <c r="C8" s="3" t="s">
         <v>41</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="C10" s="3" t="s">
         <v>41</v>
       </c>
@@ -1673,6 +1908,9 @@
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="B11" s="15" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
@@ -1697,6 +1935,9 @@
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="B14" s="15" t="s">
+        <v>119</v>
+      </c>
       <c r="C14" s="8" t="s">
         <v>41</v>
       </c>
@@ -1708,8 +1949,11 @@
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="B15" s="15" t="s">
+        <v>119</v>
+      </c>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>6</v>
@@ -1719,6 +1963,9 @@
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="B16" s="15" t="s">
+        <v>119</v>
+      </c>
       <c r="C16" s="3" t="s">
         <v>40</v>
       </c>
@@ -1730,6 +1977,12 @@
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D17" s="3" t="s">
         <v>6</v>
       </c>
@@ -1774,6 +2027,11 @@
       </c>
       <c r="D20" s="3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2097,7 +2355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2160,4 +2418,53 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="58.9453125" style="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="28.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+    </row>
+    <row r="2" spans="1:3" ht="47.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Doku ergänzt/korrigiert. Präsi vorbereitet
</commit_message>
<xml_diff>
--- a/Projekt Dokumente/Projektsteuerung.xlsx
+++ b/Projekt Dokumente/Projektsteuerung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="14160" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="14160" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitefassung" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="124">
   <si>
     <t>Wer</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Dauer [h]</t>
   </si>
   <si>
-    <t>Ifanger Reto</t>
-  </si>
-  <si>
     <t>Hartmann Peter</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>I18N mit Xamarin</t>
   </si>
   <si>
-    <t>Abkläruen/Risikominimierung</t>
-  </si>
-  <si>
     <t>In Arbeit</t>
   </si>
   <si>
@@ -403,6 +397,12 @@
   </si>
   <si>
     <t>Primärer Use-Case f. Android im UI realisieren</t>
+  </si>
+  <si>
+    <t>Infanger Reto</t>
+  </si>
+  <si>
+    <t>Abklärungen/Risikominimierung</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -533,6 +533,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -542,9 +548,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
@@ -552,9 +555,6 @@
   </cellStyles>
   <dxfs count="31">
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -635,6 +635,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -666,62 +669,62 @@
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" name="Wer" dataDxfId="28"/>
-    <tableColumn id="2" name="Was" dataDxfId="0"/>
-    <tableColumn id="6" name="Typ" dataDxfId="27"/>
-    <tableColumn id="3" name="Wann" dataDxfId="26"/>
-    <tableColumn id="4" name="Dauer [h]" dataDxfId="25"/>
+    <tableColumn id="2" name="Was" dataDxfId="27"/>
+    <tableColumn id="6" name="Typ" dataDxfId="26"/>
+    <tableColumn id="3" name="Wann" dataDxfId="25"/>
+    <tableColumn id="4" name="Dauer [h]" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A2:D25" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A2:D25" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A2:D25"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Was" dataDxfId="22"/>
-    <tableColumn id="3" name="Typ" dataDxfId="21"/>
-    <tableColumn id="5" name="Status" dataDxfId="20"/>
-    <tableColumn id="4" name="Wer" dataDxfId="19"/>
+    <tableColumn id="1" name="Was" dataDxfId="21"/>
+    <tableColumn id="3" name="Typ" dataDxfId="20"/>
+    <tableColumn id="5" name="Status" dataDxfId="19"/>
+    <tableColumn id="4" name="Wer" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A2:B24" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A2:B24" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A2:B24"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Name" dataDxfId="16"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="15"/>
+    <tableColumn id="1" name="Name" dataDxfId="15"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:E24" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:E24" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A2:E24"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="12"/>
-    <tableColumn id="2" name="Muss/Soll/Kann" dataDxfId="11"/>
-    <tableColumn id="3" name="Beschreibung" dataDxfId="10"/>
-    <tableColumn id="4" name="Status" dataDxfId="9"/>
-    <tableColumn id="5" name="Bemerkungen" dataDxfId="8"/>
+    <tableColumn id="1" name="#" dataDxfId="11"/>
+    <tableColumn id="2" name="Muss/Soll/Kann" dataDxfId="10"/>
+    <tableColumn id="3" name="Beschreibung" dataDxfId="9"/>
+    <tableColumn id="4" name="Status" dataDxfId="8"/>
+    <tableColumn id="5" name="Bemerkungen" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle6" displayName="Tabelle6" ref="A2:E33" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle6" displayName="Tabelle6" ref="A2:E33" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A2:E33"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#1" dataDxfId="5"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="4"/>
-    <tableColumn id="3" name="Finder" dataDxfId="3"/>
-    <tableColumn id="4" name="Status" dataDxfId="2"/>
-    <tableColumn id="5" name="Bemerkungen" dataDxfId="1"/>
+    <tableColumn id="1" name="#1" dataDxfId="4"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="3"/>
+    <tableColumn id="3" name="Finder" dataDxfId="2"/>
+    <tableColumn id="4" name="Status" dataDxfId="1"/>
+    <tableColumn id="5" name="Bemerkungen" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1026,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1042,12 +1045,12 @@
   <sheetData>
     <row r="1" spans="1:5" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="14"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="15" t="s">
@@ -1057,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
@@ -1068,13 +1071,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3" s="7">
         <v>43052</v>
@@ -1085,13 +1088,13 @@
     </row>
     <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D4" s="7">
         <v>43053</v>
@@ -1102,13 +1105,13 @@
     </row>
     <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="7">
         <v>43054</v>
@@ -1119,13 +1122,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="7">
         <v>43059</v>
@@ -1136,13 +1139,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="7">
         <v>43064</v>
@@ -1153,13 +1156,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="15" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="7">
         <v>43064</v>
@@ -1170,13 +1173,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="7">
         <v>43064</v>
@@ -1187,13 +1190,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="7">
         <v>43064</v>
@@ -1204,13 +1207,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="7">
         <v>43065</v>
@@ -1221,13 +1224,13 @@
     </row>
     <row r="12" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="7">
         <v>43069</v>
@@ -1238,13 +1241,13 @@
     </row>
     <row r="13" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D13" s="7">
         <v>43070</v>
@@ -1255,13 +1258,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" s="7">
         <v>43070</v>
@@ -1271,14 +1274,14 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="15" t="s">
-        <v>4</v>
+      <c r="A15" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D15" s="7">
         <v>43070</v>
@@ -1289,13 +1292,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D16" s="7">
         <v>43071</v>
@@ -1306,13 +1309,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D17" s="7">
         <v>43072</v>
@@ -1322,14 +1325,14 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="15" t="s">
-        <v>4</v>
+      <c r="A18" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D18" s="7">
         <v>43072</v>
@@ -1340,13 +1343,13 @@
     </row>
     <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D19" s="7">
         <v>43072</v>
@@ -1357,13 +1360,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D20" s="7">
         <v>43073</v>
@@ -1374,13 +1377,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D21" s="7">
         <v>43073</v>
@@ -1390,14 +1393,14 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="15" t="s">
-        <v>4</v>
+      <c r="A22" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D22" s="7">
         <v>43073</v>
@@ -1408,13 +1411,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D23" s="7">
         <v>43074</v>
@@ -1424,14 +1427,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="15" t="s">
-        <v>4</v>
+      <c r="A24" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D24" s="7">
         <v>43074</v>
@@ -1442,13 +1445,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D25" s="7">
         <v>43075</v>
@@ -1458,14 +1461,14 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="15" t="s">
-        <v>4</v>
+      <c r="A26" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D26" s="7">
         <v>43075</v>
@@ -1476,13 +1479,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D27" s="7">
         <v>43076</v>
@@ -1493,13 +1496,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D28" s="7">
         <v>43076</v>
@@ -1509,14 +1512,14 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="15" t="s">
-        <v>4</v>
+      <c r="A29" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D29" s="7">
         <v>43076</v>
@@ -1527,13 +1530,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D30" s="7">
         <v>43077</v>
@@ -1636,7 +1639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1648,95 +1651,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="A1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1744,12 +1747,12 @@
         <v>0.5</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1764,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1777,22 +1780,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="A1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>0</v>
@@ -1800,238 +1803,253 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>41</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
+      <c r="D4" s="16" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>41</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>41</v>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>4</v>
+        <v>39</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>41</v>
+      <c r="D12" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>4</v>
+        <v>38</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2063,32 +2081,32 @@
   <sheetData>
     <row r="1" spans="1:2" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2119,25 +2137,25 @@
   <sheetData>
     <row r="1" spans="1:5" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2145,10 +2163,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2156,10 +2174,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2167,10 +2185,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2178,10 +2196,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2189,10 +2207,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2200,7 +2218,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2208,10 +2226,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2219,10 +2237,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2230,10 +2248,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2241,10 +2259,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2252,10 +2270,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2263,10 +2281,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2274,10 +2292,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2285,10 +2303,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2296,10 +2314,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -2307,10 +2325,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -2370,26 +2388,26 @@
   <sheetData>
     <row r="1" spans="1:5" ht="28.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2397,10 +2415,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2408,7 +2426,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2424,40 +2442,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="58.9453125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="58.9453125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:3" ht="47.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-    </row>
-    <row r="2" spans="1:3" ht="47.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="19" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="19" t="s">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="17" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="19" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>